<commit_message>
Account TC 01 02 03
</commit_message>
<xml_diff>
--- a/automation/Repository/Accounts.xlsx
+++ b/automation/Repository/Accounts.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18690" windowHeight="4940"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13360" windowHeight="2830"/>
   </bookViews>
   <sheets>
     <sheet name="TC01_02_03" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>Status</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>ABC</t>
+  </si>
+  <si>
+    <t>*</t>
   </si>
 </sst>
 </file>
@@ -86,10 +89,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -370,10 +374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -415,6 +419,52 @@
         <v>8</v>
       </c>
     </row>
+    <row r="3" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B4" s="3">
+        <v>123</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>